<commit_message>
Added new board order details.
</commit_message>
<xml_diff>
--- a/Eagle/BMS/battery_monitor_6803-2_Rev3_Rev4-bom.xlsx
+++ b/Eagle/BMS/battery_monitor_6803-2_Rev3_Rev4-bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="282" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="268" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="204">
   <si>
     <t>Order list for /home/clayauld/Documents/Seafile/UAF/ITEST/ITEST Eagle/BMS/battery_monitor_6803-2_Rev4.sch</t>
   </si>
   <si>
     <t>Exported from EAGLE with DesignLink</t>
+  </si>
+  <si>
+    <t>Parts for 3 boards</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -733,10 +736,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -778,903 +781,826 @@
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="K6" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>48000</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S5" s="0" t="n">
-        <v>603</v>
-      </c>
-      <c r="T5" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>35812</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>0.086</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>201</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>5317</v>
+        <v>48000</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>1.02</v>
+        <v>0.016</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>8482</v>
+        <v>35812</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0.015</v>
+        <v>0.086</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>54</v>
+        <v>34</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>58</v>
+        <v>40</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>115</v>
+        <v>5317</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>224</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>0.021</v>
+        <v>1.02</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q9" s="0" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>2599</v>
+        <v>8482</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0.502</v>
+        <v>0.015</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="N10" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>56</v>
+      </c>
       <c r="C11" s="0" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.101</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>603</v>
+        <v>224</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>81</v>
+        <v>64</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>85</v>
+        <v>69</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>0</v>
+        <v>2599</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0.126</v>
+        <v>0.502</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="O12" s="0" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>2952</v>
+        <v>20</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0.169</v>
+        <v>0.101</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>100</v>
+        <v>79</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>603</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>102</v>
+        <v>81</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>1742</v>
+        <v>0</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.56</v>
+        <v>0.126</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>112</v>
+        <v>92</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>64</v>
+        <v>2952</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>8.61</v>
+        <v>0.169</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="O15" s="0" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>3110</v>
+        <v>1742</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0.009</v>
+        <v>0.56</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>134</v>
+        <v>112</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>100</v>
+        <v>3</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>20035</v>
+        <v>64</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0.008</v>
+        <v>8.61</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N17" s="0" t="n">
-        <v>201</v>
+        <v>121</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>6964</v>
+        <v>3110</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0.003</v>
+        <v>0.009</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>148</v>
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>4003</v>
+        <v>20035</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0.011</v>
+        <v>0.008</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>157</v>
+        <v>141</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>470</v>
+        <v>30</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>159</v>
+        <v>144</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>129</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>4890</v>
+        <v>6964</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0.071</v>
+        <v>0.003</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="M20" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="M20" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="N20" s="0" t="n">
-        <v>603</v>
+      <c r="N20" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>166</v>
+        <v>151</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>152</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>2513</v>
+        <v>4003</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0.003</v>
+        <v>0.011</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>171</v>
+      <c r="B22" s="1" t="n">
+        <v>470</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>160</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>1214</v>
+        <v>4890</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>0.099</v>
+        <v>0.071</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="O22" s="0" t="s">
-        <v>180</v>
+        <v>164</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>603</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>2513</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>1214</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O24" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R23" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="S23" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="T23" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="U23" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>338</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <v>0.465</v>
-      </c>
-      <c r="L24" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="N24" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="O24" s="0" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,19 +1608,101 @@
         <v>3</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="T25" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="U25" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="O26" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C25" s="0" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="C27" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="D27" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="E27" s="0" t="s">
         <v>202</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>